<commit_message>
New fields are updated in the excel sheet
Consolidate all the servers and environments and create a single record in the excel sheet and pass it to Ansible playbook.
</commit_message>
<xml_diff>
--- a/Server_Inventory_Linux.xlsx
+++ b/Server_Inventory_Linux.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\166058\Downloads\Test_XLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\166058\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Server_Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,34 +24,103 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Dev123</t>
-  </si>
-  <si>
-    <t>Dev456</t>
-  </si>
-  <si>
-    <t>Dev789</t>
-  </si>
-  <si>
-    <t>Dev321</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>CI</t>
   </si>
   <si>
     <t>Release_date</t>
   </si>
   <si>
-    <t>Configuration_Item</t>
+    <t>Affected_CIs</t>
+  </si>
+  <si>
+    <t>Short_Description</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Assigned_Group</t>
+  </si>
+  <si>
+    <t>Assigned_To</t>
+  </si>
+  <si>
+    <t>Change_Coordinator</t>
+  </si>
+  <si>
+    <t>Technical_Approver</t>
+  </si>
+  <si>
+    <t>Patching_Type</t>
+  </si>
+  <si>
+    <t>Implemention_Plan</t>
+  </si>
+  <si>
+    <t>BackoutPlan</t>
+  </si>
+  <si>
+    <t>ValidationPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development </t>
+  </si>
+  <si>
+    <t>CH3TR019845;CH3PR016586;CH3BR015586;CH3AR016586</t>
+  </si>
+  <si>
+    <t>Development  |Linux Patching</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>PFA</t>
+  </si>
+  <si>
+    <t>CH3DP020661;CH3CP123654;CH3UP136591</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>CAB Approval</t>
+  </si>
+  <si>
+    <t>Active Update</t>
+  </si>
+  <si>
+    <t>3Com DMI Agent</t>
+  </si>
+  <si>
+    <t>Luke Wilson</t>
+  </si>
+  <si>
+    <t>.Bart Hachey</t>
+  </si>
+  <si>
+    <t>Production</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,22 +128,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF343D47"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -84,40 +160,58 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,60 +492,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4">
-        <v>43475</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4">
+        <v>43467.875</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>43476</v>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4">
+        <v>43470.875</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>43477</v>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4">
+        <v>43467.875</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>43478</v>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4">
+        <v>43470.875</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43467.875</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://dev34680.service-now.com/cmdb_ci.do?sys_id=46d0bbfba9fe19810107f67241a48948"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://dev34680.service-now.com/cmdb_ci.do?sys_id=46d0bbfba9fe19810107f67241a48948"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>